<commit_message>
updating webdev grade calcuator to use the APS PIP about quality points
</commit_message>
<xml_diff>
--- a/source/sections/ite140/goals/data/WebDev_Grade_Calculator.xlsx
+++ b/source/sections/ite140/goals/data/WebDev_Grade_Calculator.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopher.jones/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopher.jones/Documents/code/gctaa_website/source/sections/ite140/goals/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F6CBC0-26AD-DD49-970B-18C538A5EFF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0993EB7B-DD2A-D147-8685-D8D4B49722DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29480" yWindow="360" windowWidth="34880" windowHeight="15780" xr2:uid="{DF04ADF1-1843-D340-BFC3-C90B9EF3C228}"/>
+    <workbookView xWindow="29480" yWindow="360" windowWidth="34880" windowHeight="16280" activeTab="1" xr2:uid="{DF04ADF1-1843-D340-BFC3-C90B9EF3C228}"/>
   </bookViews>
   <sheets>
     <sheet name="Explanation" sheetId="9" r:id="rId1"/>
@@ -23,14 +23,15 @@
   </sheets>
   <definedNames>
     <definedName name="Letter">GradeTable!$B$2:$E$10</definedName>
+    <definedName name="Letter_to_QP">GradeTable!$D$2:$E$10</definedName>
     <definedName name="Q1_final">'Q1'!$K$6</definedName>
     <definedName name="Q2_final">'Q2'!$K$6</definedName>
     <definedName name="Q3_final">'Q3'!$K$6</definedName>
     <definedName name="Q4_final">'Q4'!$K$6</definedName>
     <definedName name="QP">GradeTable!$H$2:$I$10</definedName>
-    <definedName name="Semester_1">Summary!$F$9</definedName>
-    <definedName name="Semester_2">Summary!$F$10</definedName>
-    <definedName name="Year">Summary!$F$11</definedName>
+    <definedName name="Semester_1">Summary!$C$9</definedName>
+    <definedName name="Semester_2">Summary!$C$10</definedName>
+    <definedName name="Year">Summary!$C$11</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,8 +53,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={906044AC-A2F4-2D40-B6C1-EA4F4052757D}</author>
+  </authors>
+  <commentList>
+    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{906044AC-A2F4-2D40-B6C1-EA4F4052757D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This is just whatever is better from the two rows above. I used vlookups into the grade table to turn the letter grades into numeric values and compare them.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="66">
   <si>
     <t>Assignment Name</t>
   </si>
@@ -67,9 +86,6 @@
     <t>Points Earned</t>
   </si>
   <si>
-    <t>Classwork</t>
-  </si>
-  <si>
     <t>Q1</t>
   </si>
   <si>
@@ -82,12 +98,6 @@
     <t>Q4</t>
   </si>
   <si>
-    <t>Project</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -253,14 +263,20 @@
     <t>Semeser 2 Final</t>
   </si>
   <si>
-    <t>Year Final</t>
+    <t>Year Final - QP</t>
+  </si>
+  <si>
+    <t>Year Final - Numeric</t>
+  </si>
+  <si>
+    <t>Official Final Grade</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -295,6 +311,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -441,7 +463,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -472,17 +494,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -494,30 +512,21 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="5">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -588,8 +597,8 @@
         <xdr:to>
           <xdr:col>8</xdr:col>
           <xdr:colOff>165100</xdr:colOff>
-          <xdr:row>28</xdr:row>
-          <xdr:rowOff>152400</xdr:rowOff>
+          <xdr:row>29</xdr:row>
+          <xdr:rowOff>139700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -599,7 +608,7 @@
                   <a14:compatExt spid="_x0000_s8194"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94FE9595-4D26-DAAA-2CF8-51D43077AD3C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002200000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -620,23 +629,10 @@
               <a:solidFill>
                 <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
-              <a:tailEnd type="none" w="med" len="med"/>
+              <a:tailEnd/>
             </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -648,7 +644,9 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Jones, Christopher" id="{EFCAD197-AF9F-5546-B0A0-9329CFFCBBC4}" userId="Jones, Christopher" providerId="None"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -946,11 +944,19 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C13" dT="2024-09-10T19:37:27.25" personId="{EFCAD197-AF9F-5546-B0A0-9329CFFCBBC4}" id="{906044AC-A2F4-2D40-B6C1-EA4F4052757D}">
+    <text>This is just whatever is better from the two rows above. I used vlookups into the grade table to turn the letter grades into numeric values and compare them.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63BD9A3D-4790-054A-B773-8A652CC11E40}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
@@ -975,8 +981,8 @@
               <to>
                 <xdr:col>8</xdr:col>
                 <xdr:colOff>165100</xdr:colOff>
-                <xdr:row>28</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
+                <xdr:row>29</xdr:row>
+                <xdr:rowOff>139700</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -991,252 +997,237 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80114B9B-8AD1-3442-BDFB-62FDB7C39312}">
-  <dimension ref="B1:J11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80114B9B-8AD1-3442-BDFB-62FDB7C39312}">
+  <dimension ref="B1:H13"/>
   <sheetViews>
-    <sheetView zoomScale="232" zoomScaleNormal="232" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScale="232" zoomScaleNormal="232" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.83203125" customWidth="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="0" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.6640625" customWidth="1"/>
-    <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" style="13"/>
+    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="13" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B2" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="14" t="s">
+    <row r="1" spans="2:8" ht="13" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B2" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="J2" s="29"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B3" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="17">
-        <f>'Q1'!C2</f>
-        <v>0</v>
-      </c>
-      <c r="D3" s="17" t="e">
-        <f>'Q1'!#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E3" s="17">
-        <f>'Q1'!F2</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="18">
+      <c r="G2" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="25"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B3" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="16">
         <f>Q1_final</f>
         <v>0.92726666666666668</v>
       </c>
-      <c r="G3" s="19" t="str">
-        <f>VLOOKUP(F3*100,Letter,3)</f>
+      <c r="D3" s="30" t="str">
+        <f t="shared" ref="D3:D11" si="0">VLOOKUP(C3*100,Letter,3)</f>
         <v>A</v>
       </c>
-      <c r="I3" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="J3" s="31">
+      <c r="E3" s="17">
+        <f>VLOOKUP(D3,Letter_to_QP,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="27">
         <v>0.4</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="17" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D4" s="17" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E4" s="17" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F4" s="18">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B4" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="16">
         <f>Q2_final</f>
         <v>0.90966666666666662</v>
       </c>
-      <c r="G4" s="19" t="str">
-        <f>VLOOKUP(F4*100,Letter,3)</f>
+      <c r="D4" s="30" t="str">
+        <f t="shared" si="0"/>
         <v>A</v>
       </c>
-      <c r="I4" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="J4" s="33">
+      <c r="E4" s="17">
+        <f>VLOOKUP(D4,Letter_to_QP,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="H4" s="29">
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B5" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="18">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="16">
         <v>0.85</v>
       </c>
-      <c r="G5" s="19" t="str">
-        <f>VLOOKUP(F5*100,Letter,3)</f>
+      <c r="D5" s="30" t="str">
+        <f t="shared" si="0"/>
         <v>B</v>
       </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B6" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="17" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D6" s="17" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E6" s="17" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F6" s="18">
+      <c r="E5" s="17">
+        <f>VLOOKUP(D5,Letter_to_QP,2,FALSE)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="16">
         <f>Q3_final</f>
         <v>0.9127333333333334</v>
       </c>
-      <c r="G6" s="19" t="str">
-        <f>VLOOKUP(F6*100,Letter,3)</f>
+      <c r="D6" s="30" t="str">
+        <f t="shared" si="0"/>
         <v>A</v>
       </c>
-      <c r="I6" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="J6" s="29"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B7" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="17" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D7" s="17" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E7" s="17" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F7" s="18">
+      <c r="E6" s="17">
+        <f>VLOOKUP(D6,Letter_to_QP,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" s="25"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="16">
         <f>Q4_final</f>
         <v>0.9207333333333334</v>
       </c>
-      <c r="G7" s="19" t="str">
-        <f>VLOOKUP(F7*100,Letter,3)</f>
+      <c r="D7" s="30" t="str">
+        <f t="shared" si="0"/>
         <v>A</v>
       </c>
-      <c r="I7" s="32" t="s">
+      <c r="E7" s="17">
+        <f>VLOOKUP(D7,Letter_to_QP,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" s="29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="22">
+        <v>0</v>
+      </c>
+      <c r="D8" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>E</v>
+      </c>
+      <c r="E8" s="23">
+        <f>VLOOKUP(D8,Letter_to_QP,2,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="16">
+        <f>C3*H3+C4*H3+C5*H4</f>
+        <v>0.90477333333333343</v>
+      </c>
+      <c r="D9" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+      <c r="E9" s="30"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="J7" s="33">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="26">
-        <v>0</v>
-      </c>
-      <c r="G8" s="27" t="str">
-        <f>VLOOKUP(F8*100,Letter,3)</f>
-        <v>E</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="16" t="s">
+      <c r="C10" s="16">
+        <f>C6*H3+C7*H3+C8*H4</f>
+        <v>0.73338666666666674</v>
+      </c>
+      <c r="D10" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>C</v>
+      </c>
+      <c r="E10" s="30"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="18">
-        <f>F3*J3+F4*J3+F5*J4</f>
-        <v>0.90477333333333343</v>
-      </c>
-      <c r="G9" s="19" t="str">
-        <f>VLOOKUP(F9*100,Letter,3)</f>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="16" t="s">
+      <c r="C11" s="16">
+        <f>C9*H7+C10*H7</f>
+        <v>0.81908000000000003</v>
+      </c>
+      <c r="D11" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>B</v>
+      </c>
+      <c r="E11" s="30"/>
+    </row>
+    <row r="12" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="21">
+        <f>(E3*H3+E4*H3+E5*H4)*H7+(E6*H3+E7*H3+E8*H4)*H7</f>
+        <v>3.5</v>
+      </c>
+      <c r="D12" s="23" t="str">
+        <f>VLOOKUP(C12,QP,2)</f>
+        <v>B+</v>
+      </c>
+      <c r="E12" s="30"/>
+    </row>
+    <row r="13" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="18">
-        <f>F6*J3+F7*J3+F8*J4</f>
-        <v>0.73338666666666674</v>
-      </c>
-      <c r="G10" s="19" t="str">
-        <f>VLOOKUP(F10*100,Letter,3)</f>
-        <v>C</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B11" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="22">
-        <f>F9*J7+F10*J7</f>
-        <v>0.81908000000000003</v>
-      </c>
-      <c r="G11" s="23" t="str">
-        <f>VLOOKUP(F11*100,Letter,3)</f>
-        <v>B</v>
+      <c r="C13" s="19" t="str">
+        <f>IF(VLOOKUP(D11,Letter_to_QP,2,FALSE)&gt;VLOOKUP(D12,Letter_to_QP,2,FALSE),D11,D12)</f>
+        <v>B+</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D11:D12">
+    <cfRule type="top10" dxfId="0" priority="1" rank="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1266,18 +1257,18 @@
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.2">
       <c r="M1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B2" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M2">
         <f>SMALL(C:C,1)</f>
@@ -1304,9 +1295,9 @@
         <v>3</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="13">
+        <v>23</v>
+      </c>
+      <c r="K3" s="12">
         <f>(SUM(C:C)-SUM(M:M))/(100*(COUNT(C:C)-5))</f>
         <v>0.87133333333333329</v>
       </c>
@@ -1317,13 +1308,13 @@
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <v>79</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F4">
         <v>88</v>
@@ -1336,9 +1327,9 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" s="13">
+        <v>24</v>
+      </c>
+      <c r="K4" s="12">
         <f>SUM(H4:H7)/SUM(G4:G7)</f>
         <v>0.94124999999999992</v>
       </c>
@@ -1349,13 +1340,13 @@
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C5">
         <v>79</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F5">
         <v>100</v>
@@ -1374,13 +1365,13 @@
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <v>89</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F6">
         <v>83</v>
@@ -1393,9 +1384,9 @@
         <v>4.1499999999999995</v>
       </c>
       <c r="J6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K6" s="13">
+        <v>8</v>
+      </c>
+      <c r="K6" s="12">
         <f>0.8*K4+0.2*K3</f>
         <v>0.92726666666666668</v>
       </c>
@@ -1406,18 +1397,18 @@
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C7">
         <v>94</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F7">
         <v>98</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7">
         <v>15</v>
       </c>
       <c r="H7">
@@ -1427,7 +1418,7 @@
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C8">
         <v>86</v>
@@ -1435,7 +1426,7 @@
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C9">
         <v>71</v>
@@ -1443,7 +1434,7 @@
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C10">
         <v>77</v>
@@ -1451,7 +1442,7 @@
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C11">
         <v>97</v>
@@ -1459,7 +1450,7 @@
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C12">
         <v>81</v>
@@ -1467,7 +1458,7 @@
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C13">
         <v>69</v>
@@ -1475,7 +1466,7 @@
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C14">
         <v>84</v>
@@ -1483,7 +1474,7 @@
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C15">
         <v>71</v>
@@ -1491,7 +1482,7 @@
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C16">
         <v>75</v>
@@ -1499,7 +1490,7 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C17">
         <v>63</v>
@@ -1507,7 +1498,7 @@
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C18">
         <v>63</v>
@@ -1515,7 +1506,7 @@
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C19">
         <v>94</v>
@@ -1523,7 +1514,7 @@
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C20">
         <v>98</v>
@@ -1531,7 +1522,7 @@
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C21">
         <v>91</v>
@@ -1539,7 +1530,7 @@
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C22">
         <v>91</v>
@@ -1547,7 +1538,7 @@
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C23">
         <v>92</v>
@@ -1556,7 +1547,7 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="C4:C23">
-    <cfRule type="top10" dxfId="5" priority="1" bottom="1" rank="5"/>
+    <cfRule type="top10" dxfId="4" priority="1" bottom="1" rank="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1585,18 +1576,18 @@
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.2">
       <c r="M1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B2" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M2">
         <f>SMALL(C:C,1)</f>
@@ -1623,9 +1614,9 @@
         <v>3</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="13">
+        <v>23</v>
+      </c>
+      <c r="K3" s="12">
         <f>(SUM(C:C)-SUM(M:M))/(100*(COUNT(C:C)-5))</f>
         <v>0.78333333333333333</v>
       </c>
@@ -1636,13 +1627,13 @@
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <v>99</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F4">
         <v>88</v>
@@ -1655,9 +1646,9 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" s="13">
+        <v>24</v>
+      </c>
+      <c r="K4" s="12">
         <f>SUM(H4:H7)/SUM(G4:G7)</f>
         <v>0.94124999999999992</v>
       </c>
@@ -1668,13 +1659,13 @@
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C5">
         <v>67</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F5">
         <v>100</v>
@@ -1693,13 +1684,13 @@
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <v>81</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F6">
         <v>83</v>
@@ -1712,9 +1703,9 @@
         <v>4.1499999999999995</v>
       </c>
       <c r="J6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K6" s="13">
+        <v>8</v>
+      </c>
+      <c r="K6" s="12">
         <f>0.8*K4+0.2*K3</f>
         <v>0.90966666666666662</v>
       </c>
@@ -1725,18 +1716,18 @@
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C7">
         <v>100</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F7">
         <v>98</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7">
         <v>15</v>
       </c>
       <c r="H7">
@@ -1746,7 +1737,7 @@
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C8">
         <v>67</v>
@@ -1754,7 +1745,7 @@
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C9">
         <v>63</v>
@@ -1762,7 +1753,7 @@
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C10">
         <v>81</v>
@@ -1770,7 +1761,7 @@
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C11">
         <v>93</v>
@@ -1778,7 +1769,7 @@
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C12">
         <v>63</v>
@@ -1786,7 +1777,7 @@
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C13">
         <v>61</v>
@@ -1794,7 +1785,7 @@
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C14">
         <v>70</v>
@@ -1802,7 +1793,7 @@
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C15">
         <v>62</v>
@@ -1810,7 +1801,7 @@
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C16">
         <v>65</v>
@@ -1818,7 +1809,7 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C17">
         <v>63</v>
@@ -1826,7 +1817,7 @@
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C18">
         <v>79</v>
@@ -1834,7 +1825,7 @@
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C19">
         <v>68</v>
@@ -1842,7 +1833,7 @@
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C20">
         <v>91</v>
@@ -1850,7 +1841,7 @@
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C21">
         <v>68</v>
@@ -1858,7 +1849,7 @@
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C22">
         <v>79</v>
@@ -1866,7 +1857,7 @@
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C23">
         <v>67</v>
@@ -1874,7 +1865,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C4:C23">
-    <cfRule type="top10" dxfId="4" priority="1" bottom="1" rank="5"/>
+    <cfRule type="top10" dxfId="3" priority="1" bottom="1" rank="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1904,18 +1895,18 @@
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.2">
       <c r="M1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B2" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M2">
         <f>SMALL(C:C,1)</f>
@@ -1942,9 +1933,9 @@
         <v>3</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="13">
+        <v>23</v>
+      </c>
+      <c r="K3" s="12">
         <f>(SUM(C:C)-SUM(M:M))/(100*(COUNT(C:C)-5))</f>
         <v>0.79866666666666664</v>
       </c>
@@ -1955,13 +1946,13 @@
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <v>85</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F4">
         <v>88</v>
@@ -1974,9 +1965,9 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" s="13">
+        <v>24</v>
+      </c>
+      <c r="K4" s="12">
         <f>SUM(H4:H7)/SUM(G4:G7)</f>
         <v>0.94124999999999992</v>
       </c>
@@ -1987,13 +1978,13 @@
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C5">
         <v>65</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F5">
         <v>100</v>
@@ -2012,13 +2003,13 @@
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <v>96</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F6">
         <v>83</v>
@@ -2031,9 +2022,9 @@
         <v>4.1499999999999995</v>
       </c>
       <c r="J6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K6" s="13">
+        <v>8</v>
+      </c>
+      <c r="K6" s="12">
         <f>0.8*K4+0.2*K3</f>
         <v>0.9127333333333334</v>
       </c>
@@ -2044,18 +2035,18 @@
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C7">
         <v>68</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F7">
         <v>98</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7">
         <v>15</v>
       </c>
       <c r="H7">
@@ -2065,7 +2056,7 @@
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C8">
         <v>64</v>
@@ -2073,7 +2064,7 @@
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C9">
         <v>83</v>
@@ -2081,7 +2072,7 @@
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C10">
         <v>76</v>
@@ -2089,7 +2080,7 @@
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C11">
         <v>69</v>
@@ -2097,7 +2088,7 @@
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C12">
         <v>77</v>
@@ -2105,7 +2096,7 @@
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C13">
         <v>66</v>
@@ -2113,7 +2104,7 @@
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C14">
         <v>63</v>
@@ -2121,7 +2112,7 @@
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C15">
         <v>67</v>
@@ -2129,7 +2120,7 @@
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C16">
         <v>79</v>
@@ -2137,7 +2128,7 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C17">
         <v>92</v>
@@ -2145,7 +2136,7 @@
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C18">
         <v>68</v>
@@ -2153,7 +2144,7 @@
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C19">
         <v>84</v>
@@ -2161,7 +2152,7 @@
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C20">
         <v>65</v>
@@ -2169,7 +2160,7 @@
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C21">
         <v>84</v>
@@ -2177,7 +2168,7 @@
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C22">
         <v>94</v>
@@ -2185,7 +2176,7 @@
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C23">
         <v>76</v>
@@ -2193,7 +2184,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C4:C23">
-    <cfRule type="top10" dxfId="1" priority="1" bottom="1" rank="5"/>
+    <cfRule type="top10" dxfId="2" priority="1" bottom="1" rank="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2223,18 +2214,18 @@
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.2">
       <c r="M1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B2" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M2">
         <f>SMALL(C:C,1)</f>
@@ -2261,9 +2252,9 @@
         <v>3</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="13">
+        <v>23</v>
+      </c>
+      <c r="K3" s="12">
         <f>(SUM(C:C)-SUM(M:M))/(100*(COUNT(C:C)-5))</f>
         <v>0.83866666666666667</v>
       </c>
@@ -2274,13 +2265,13 @@
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C4">
         <v>100</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F4">
         <v>88</v>
@@ -2293,9 +2284,9 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" s="13">
+        <v>24</v>
+      </c>
+      <c r="K4" s="12">
         <f>SUM(H4:H7)/SUM(G4:G7)</f>
         <v>0.94124999999999992</v>
       </c>
@@ -2306,13 +2297,13 @@
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C5">
         <v>61</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F5">
         <v>100</v>
@@ -2331,13 +2322,13 @@
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <v>65</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F6">
         <v>83</v>
@@ -2350,9 +2341,9 @@
         <v>4.1499999999999995</v>
       </c>
       <c r="J6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K6" s="13">
+        <v>8</v>
+      </c>
+      <c r="K6" s="12">
         <f>0.8*K4+0.2*K3</f>
         <v>0.9207333333333334</v>
       </c>
@@ -2363,18 +2354,18 @@
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C7">
         <v>61</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F7">
         <v>98</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7">
         <v>15</v>
       </c>
       <c r="H7">
@@ -2384,7 +2375,7 @@
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C8">
         <v>74</v>
@@ -2392,7 +2383,7 @@
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C9">
         <v>94</v>
@@ -2400,7 +2391,7 @@
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C10">
         <v>93</v>
@@ -2408,7 +2399,7 @@
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C11">
         <v>68</v>
@@ -2416,7 +2407,7 @@
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C12">
         <v>66</v>
@@ -2424,7 +2415,7 @@
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C13">
         <v>83</v>
@@ -2432,7 +2423,7 @@
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C14">
         <v>88</v>
@@ -2440,7 +2431,7 @@
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C15">
         <v>78</v>
@@ -2448,7 +2439,7 @@
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C16">
         <v>99</v>
@@ -2456,7 +2447,7 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C17">
         <v>89</v>
@@ -2464,7 +2455,7 @@
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C18">
         <v>72</v>
@@ -2472,7 +2463,7 @@
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C19">
         <v>87</v>
@@ -2480,7 +2471,7 @@
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C20">
         <v>64</v>
@@ -2488,7 +2479,7 @@
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C21">
         <v>92</v>
@@ -2496,7 +2487,7 @@
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C22">
         <v>61</v>
@@ -2504,7 +2495,7 @@
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C23">
         <v>75</v>
@@ -2512,7 +2503,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C4:C23">
-    <cfRule type="top10" dxfId="0" priority="1" bottom="1" rank="5"/>
+    <cfRule type="top10" dxfId="1" priority="1" bottom="1" rank="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2524,7 +2515,7 @@
   <dimension ref="B2:I10"/>
   <sheetViews>
     <sheetView zoomScale="178" zoomScaleNormal="178" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2540,22 +2531,22 @@
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B2" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.2">
@@ -2566,7 +2557,7 @@
         <v>59</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E3" s="7">
         <v>0</v>
@@ -2575,7 +2566,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
@@ -2586,7 +2577,7 @@
         <v>66</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E4" s="7">
         <v>1</v>
@@ -2595,7 +2586,7 @@
         <v>0.75</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
@@ -2606,7 +2597,7 @@
         <v>69</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E5" s="7">
         <v>1.5</v>
@@ -2615,7 +2606,7 @@
         <v>1.25</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
@@ -2626,7 +2617,7 @@
         <v>76</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E6" s="7">
         <v>2</v>
@@ -2635,7 +2626,7 @@
         <v>1.75</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
@@ -2646,7 +2637,7 @@
         <v>79</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E7" s="7">
         <v>2.5</v>
@@ -2655,7 +2646,7 @@
         <v>2.25</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
@@ -2666,7 +2657,7 @@
         <v>86</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E8" s="7">
         <v>3</v>
@@ -2675,7 +2666,7 @@
         <v>2.75</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.2">
@@ -2686,7 +2677,7 @@
         <v>89</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E9" s="7">
         <v>3.5</v>
@@ -2695,7 +2686,7 @@
         <v>3.25</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
@@ -2706,7 +2697,7 @@
         <v>100</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E10" s="9">
         <v>4</v>
@@ -2715,7 +2706,7 @@
         <v>3.75</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>